<commit_message>
create Lingo file and formulation  in programmig problem
</commit_message>
<xml_diff>
--- a/Secondo progetto/ese2_data.xlsx
+++ b/Secondo progetto/ese2_data.xlsx
@@ -3,24 +3,33 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C6DA6C-74F6-413D-A803-B7A0CC625845}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6A021-4470-4375-966A-A43E83BEDAFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="precess_time">Foglio1!$B$12:$K$13</definedName>
+    <definedName name="process_time">Foglio1!$B$12:$K$13</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Job</t>
   </si>
@@ -122,12 +131,21 @@
       <t>4</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Process Time </t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +164,14 @@
     <font>
       <i/>
       <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -239,6 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -519,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +729,104 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B4)</f>
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="0">SUM(C2:C4)</f>
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B5)</f>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:K13" si="1">SUM(C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>